<commit_message>
UI: Sleek minimal progress bar, summary table manual field sync, MBMC parser bugfixes
</commit_message>
<xml_diff>
--- a/MBMC/Config_MBMC.xlsx
+++ b/MBMC/Config_MBMC.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://netorg1056155-my.sharepoint.com/personal/r_sashwat_cloudextel_com/Documents/TrenchExtractor/MBMC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="59" documentId="11_F25DC773A252ABDACC10488DE9DE78A45BDE58F0" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7A7CBEE4-AFFB-4463-90CA-01BFDD5A979C}"/>
+  <xr:revisionPtr revIDLastSave="61" documentId="11_F25DC773A252ABDACC10488DE9DE78A45BDE58F0" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{46D543F1-05E3-4822-B19C-7432CB26473E}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="116">
   <si>
     <t>Intercity/Intracity- Deployment
 Intercity/intracity- O&amp;M
@@ -339,6 +339,54 @@
   </si>
   <si>
     <t>master demand note file + DB</t>
+  </si>
+  <si>
+    <t>Intercity/Intracity- Deployment Intercity/intracity- O&amp;M FTTH- Deployment FTTH-O&amp;M</t>
+  </si>
+  <si>
+    <t>Annual Rate/Pole( current DN)</t>
+  </si>
+  <si>
+    <t>HDD(PIT RATE)</t>
+  </si>
+  <si>
+    <t>Non Refundable Cost( Amount to process for payment shold be sum of 'Z' and 'AA' coulm )</t>
+  </si>
+  <si>
+    <t>REASON FOR DELAY (&gt;2 DAYS)</t>
+  </si>
+  <si>
+    <t>9600</t>
+  </si>
+  <si>
+    <t>124</t>
+  </si>
+  <si>
+    <t>1215200</t>
+  </si>
+  <si>
+    <t>Restoration Charges</t>
+  </si>
+  <si>
+    <t>218736</t>
+  </si>
+  <si>
+    <t>119040</t>
+  </si>
+  <si>
+    <t>30/04/2025</t>
+  </si>
+  <si>
+    <t>55</t>
+  </si>
+  <si>
+    <t>1552976</t>
+  </si>
+  <si>
+    <t>MIRA BHAYANDAR MUNICIPAL CORPORATION</t>
+  </si>
+  <si>
+    <t>Mira Bhayandar</t>
   </si>
 </sst>
 </file>
@@ -349,7 +397,7 @@
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="164" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -439,6 +487,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="4">
@@ -533,7 +586,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -595,6 +648,9 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -613,6 +669,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -878,10 +938,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BG14"/>
+  <dimension ref="A1:BG26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="AN1" workbookViewId="0">
+      <selection activeCell="BG6" sqref="BG6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1187,7 +1247,7 @@
       </c>
       <c r="AJ2" s="11">
         <f ca="1">TODAY()-AI2</f>
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="AK2" s="14"/>
       <c r="AL2" s="15">
@@ -1296,51 +1356,323 @@
       </c>
     </row>
     <row r="5" spans="1:59" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>75</v>
+      <c r="A5" s="22" t="s">
+        <v>100</v>
+      </c>
+      <c r="B5" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="G5" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="H5" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="I5" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="J5" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="K5" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="L5" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="M5" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="N5" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="O5" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="P5" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q5" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="R5" s="22" t="s">
+        <v>101</v>
+      </c>
+      <c r="S5" s="22" t="s">
+        <v>102</v>
+      </c>
+      <c r="T5" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="U5" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="V5" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="W5" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="X5" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y5" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z5" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA5" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB5" s="22" t="s">
+        <v>103</v>
+      </c>
+      <c r="AC5" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD5" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE5" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="AF5" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="AG5" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="AH5" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="AI5" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="AJ5" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="AK5" s="22" t="s">
+        <v>104</v>
+      </c>
+      <c r="AL5" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="AM5" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="AN5" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="AO5" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="AP5" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="AQ5" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="AR5" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="AS5" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="AT5" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="AU5" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="AV5" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="AW5" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="AX5" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="AY5" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="AZ5" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="BA5" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="BB5" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="BC5" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="BD5" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="BE5" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="BF5" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="BG5" s="22" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C6" t="s">
+        <v>61</v>
+      </c>
+      <c r="D6" t="s">
+        <v>61</v>
+      </c>
+      <c r="E6" t="s">
+        <v>62</v>
+      </c>
+      <c r="G6" t="s">
+        <v>63</v>
+      </c>
+      <c r="H6" t="s">
+        <v>64</v>
+      </c>
+      <c r="I6" t="s">
+        <v>65</v>
+      </c>
+      <c r="J6" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>105</v>
+      </c>
+      <c r="T6" t="s">
+        <v>106</v>
+      </c>
+      <c r="U6" t="s">
+        <v>106</v>
+      </c>
+      <c r="AA6" t="s">
+        <v>107</v>
+      </c>
+      <c r="AB6" t="s">
+        <v>107</v>
+      </c>
+      <c r="AC6" t="s">
+        <v>108</v>
+      </c>
+      <c r="AD6" t="s">
+        <v>109</v>
+      </c>
+      <c r="AF6" t="s">
+        <v>110</v>
+      </c>
+      <c r="AH6" t="s">
+        <v>111</v>
+      </c>
+      <c r="AI6" t="s">
+        <v>111</v>
+      </c>
+      <c r="AJ6" t="s">
+        <v>112</v>
+      </c>
+      <c r="AL6" t="s">
+        <v>113</v>
+      </c>
+      <c r="AO6" t="s">
+        <v>69</v>
+      </c>
+      <c r="AQ6" t="s">
+        <v>114</v>
+      </c>
+      <c r="AR6" t="s">
+        <v>114</v>
+      </c>
+      <c r="AS6" t="s">
+        <v>71</v>
+      </c>
+      <c r="AT6" t="s">
+        <v>72</v>
+      </c>
+      <c r="AU6" t="s">
+        <v>115</v>
+      </c>
+      <c r="AV6" t="s">
+        <v>115</v>
+      </c>
+      <c r="BC6" t="s">
+        <v>108</v>
+      </c>
+      <c r="BF6" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="7" spans="1:59" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="9" spans="1:59" x14ac:dyDescent="0.3">
-      <c r="B9" t="s">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B21" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="10" spans="1:59" x14ac:dyDescent="0.3">
-      <c r="B10" t="s">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B22" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="11" spans="1:59" x14ac:dyDescent="0.3">
-      <c r="B11" t="s">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B23" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="12" spans="1:59" x14ac:dyDescent="0.3">
-      <c r="B12" t="s">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B24" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="13" spans="1:59" x14ac:dyDescent="0.3">
-      <c r="B13" t="s">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B25" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="14" spans="1:59" x14ac:dyDescent="0.3">
-      <c r="B14" t="s">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B26" t="s">
         <v>99</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>